<commit_message>
Att dos processos de deposito, extrato, pagamento e transferencia
</commit_message>
<xml_diff>
--- a/Data/Base.xlsx
+++ b/Data/Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1e5a0122e61a6c0/Documentos/UiPath/Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC104812891D75125BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F89F8CD-427E-4818-A9D2-97FC4B8BBE31}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="11_F25DC773A252ABDACC104812891D75125BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE668CDE-7F84-4FDF-8E09-02259F8EF2CE}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="1125" windowWidth="28770" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
         <v>123</v>
       </c>
       <c r="E2">
-        <v>209.88</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
         <v>123</v>
       </c>
       <c r="E29">
-        <v>500.6</v>
+        <v>489</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajuste em retry e extrato negativo
</commit_message>
<xml_diff>
--- a/Data/Base.xlsx
+++ b/Data/Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1e5a0122e61a6c0/Documentos/UiPath/Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="11_F25DC773A252ABDACC104812891D75125BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE668CDE-7F84-4FDF-8E09-02259F8EF2CE}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC104812891D75125BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{907100CB-C722-4D1B-B69C-94ADB03C5F9A}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="1125" windowWidth="28770" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>Laura</t>
   </si>
   <si>
-    <t>Manuela</t>
-  </si>
-  <si>
     <t>Madalena</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>conta</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -500,7 +500,7 @@
         <v>123</v>
       </c>
       <c r="E2">
-        <v>510</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -517,7 +517,7 @@
         <v>123</v>
       </c>
       <c r="E3">
-        <v>1092.9100000000001</v>
+        <v>1192.9100000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,16 +576,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>108767</v>
       </c>
       <c r="D7">
-        <v>123</v>
+        <v>1101</v>
       </c>
       <c r="E7">
-        <v>8278</v>
+        <v>10278</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>108784</v>
@@ -627,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>108827</v>
@@ -712,7 +712,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>108987</v>
@@ -729,7 +729,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>109028</v>
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>109072</v>
@@ -763,7 +763,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>109119</v>
@@ -780,7 +780,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>109169</v>
@@ -797,7 +797,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>109222</v>
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>109278</v>
@@ -831,7 +831,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>109337</v>
@@ -848,7 +848,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>109399</v>
@@ -865,7 +865,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>109464</v>
@@ -882,7 +882,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>109532</v>
@@ -899,7 +899,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>109603</v>
@@ -916,7 +916,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>109677</v>
@@ -933,7 +933,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>109754</v>
@@ -950,7 +950,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>109834</v>
@@ -967,7 +967,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>109917</v>
@@ -984,7 +984,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>110003</v>

</xml_diff>